<commit_message>
fixed issue with entra/xdr total cost
..by combining the cells.
</commit_message>
<xml_diff>
--- a/costCalculator/Sentinel_cost_calculator.xlsx
+++ b/costCalculator/Sentinel_cost_calculator.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/21d5b7141008e847/Asiakirjat/Työ/Microsoft/Blog/costCalculator/v1.0/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/21d5b7141008e847/Asiakirjat/Työ/Microsoft/Blog/costCalculator/v1.01/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="867" documentId="8_{45702357-D6A7-4ABD-904D-A6F59F38FD28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{965A472E-1CF6-4B86-8D7A-6ABB8CF2FBD6}"/>
+  <xr:revisionPtr revIDLastSave="903" documentId="8_{45702357-D6A7-4ABD-904D-A6F59F38FD28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5FDC267-264A-4082-B7C9-39F0E753A3CD}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="13110" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{F636714E-48EB-4F2C-A90F-78103E777235}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{F636714E-48EB-4F2C-A90F-78103E777235}"/>
   </bookViews>
   <sheets>
     <sheet name="Usage" sheetId="7" r:id="rId1"/>
@@ -1205,13 +1205,13 @@
     <t>&gt;&gt;&gt; Data lake ingestion ($0.05) + Data lake processing ($0.10), roughly $0.15 alltogether across all data lake sources.</t>
   </si>
   <si>
-    <t>Sentinel cost calculator (unofficial) v1.0</t>
-  </si>
-  <si>
     <t>sentinel/costCalculator at main · markolauren/sentinel</t>
   </si>
   <si>
     <t>Latest version in Github:</t>
+  </si>
+  <si>
+    <t>Sentinel cost calculator (unofficial) v1.01</t>
   </si>
 </sst>
 </file>
@@ -1420,7 +1420,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1603,12 +1603,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39994506668294322"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39994506668294322"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1886,6 +1912,12 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1934,7 +1966,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ h:mm"/>
+      <numFmt numFmtId="169" formatCode="dd/mm/yyyy\ h:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -2474,10 +2506,10 @@
                   <c:v>12790.1214</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1602.1530000000002</c:v>
+                  <c:v>351.91800000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>224.87549999999996</c:v>
+                  <c:v>264.76799999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1851.6</c:v>
@@ -5409,12 +5441,12 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" s="81" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" s="88" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
@@ -5517,7 +5549,7 @@
   <dimension ref="B1:AE94"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="14.65" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
@@ -5545,7 +5577,7 @@
   <sheetData>
     <row r="1" spans="2:31" ht="25.5" x14ac:dyDescent="0.5">
       <c r="B1" s="17" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="H1" s="71" t="s">
         <v>6</v>
@@ -6150,9 +6182,9 @@
         <v>11.819999999999999</v>
       </c>
       <c r="O22" s="56"/>
-      <c r="P22" s="57">
-        <f>N22+M22+K22</f>
-        <v>1203.2301</v>
+      <c r="P22" s="99">
+        <f>N22+M22+K22+M23+N23</f>
+        <v>1296.3126</v>
       </c>
       <c r="Q22" s="20"/>
       <c r="AA22" s="4"/>
@@ -6175,7 +6207,7 @@
       <c r="F23" s="93"/>
       <c r="G23" s="40"/>
       <c r="H23" s="70">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="I23" s="70">
         <v>24</v>
@@ -6184,17 +6216,14 @@
       <c r="L23" s="56"/>
       <c r="M23" s="55">
         <f t="shared" si="3"/>
-        <v>1250.2350000000001</v>
+        <v>0</v>
       </c>
       <c r="N23" s="55">
         <f t="shared" si="4"/>
-        <v>53.189999999999984</v>
+        <v>93.082499999999982</v>
       </c>
       <c r="O23" s="56"/>
-      <c r="P23" s="57">
-        <f t="shared" ref="P23:P44" si="6">N23+M23+K23</f>
-        <v>1303.4250000000002</v>
-      </c>
+      <c r="P23" s="100"/>
       <c r="Q23" s="20"/>
       <c r="AA23" s="4"/>
       <c r="AC23" s="54" t="s">
@@ -6237,7 +6266,7 @@
       </c>
       <c r="O24" s="56"/>
       <c r="P24" s="57">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="P24:P44" si="6">N24+M24+K24</f>
         <v>39.892499999999991</v>
       </c>
       <c r="Q24" s="20"/>
@@ -6953,16 +6982,16 @@
       <c r="L46" s="56"/>
       <c r="M46" s="56">
         <f>SUM(M20:M44)</f>
-        <v>1602.1530000000002</v>
+        <v>351.91800000000001</v>
       </c>
       <c r="N46" s="56">
         <f>SUM(N20:N44)</f>
-        <v>224.87549999999996</v>
+        <v>264.76799999999997</v>
       </c>
       <c r="O46" s="56"/>
       <c r="P46" s="56">
         <f>SUM(P20:P44)</f>
-        <v>14617.149899999999</v>
+        <v>13406.8074</v>
       </c>
       <c r="Q46" s="20"/>
       <c r="Z46" s="20"/>
@@ -8618,7 +8647,7 @@
       </c>
       <c r="C85" s="55">
         <f>M46</f>
-        <v>1602.1530000000002</v>
+        <v>351.91800000000001</v>
       </c>
       <c r="D85" s="59"/>
       <c r="E85" s="59"/>
@@ -8638,7 +8667,7 @@
       </c>
       <c r="C86" s="55">
         <f>N46</f>
-        <v>224.87549999999996</v>
+        <v>264.76799999999997</v>
       </c>
       <c r="D86" s="59"/>
       <c r="E86" s="59"/>
@@ -8766,7 +8795,7 @@
       </c>
       <c r="C93" s="61">
         <f>SUM(C84:C90)</f>
-        <v>17059.749899999999</v>
+        <v>15849.4074</v>
       </c>
       <c r="D93" s="72" t="str">
         <f>C4</f>
@@ -8807,17 +8836,18 @@
       <c r="AE94" s="4"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="E0ktZiYeZcTZ54lGGXzDwVaaCLWj5txkO88DT4ZGKD9IJxABlXwIv/QfhsYDUtdZlZ8MLb+zaQrgLICRQfRgGA==" saltValue="MGUGL0J0Afn5GNn0dv/kdA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="mOTAG2jqZyb3r/Vnsrk/vY76MNEqgJDtn0MB9cLkPKBRjzheCEVLv3TUz0YCtVZgod8jkWLTlAmBfi3UXpCSLw==" saltValue="8GfV6B+dsCRN6j2MbeFflw==" spinCount="100000" sheet="1" formatRows="0"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="AE5:AE21">
     <sortCondition ref="AE5:AE21"/>
   </sortState>
-  <mergeCells count="11">
+  <mergeCells count="12">
     <mergeCell ref="F22:F23"/>
     <mergeCell ref="K22:K23"/>
     <mergeCell ref="E22:E23"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="B17:I17"/>
     <mergeCell ref="K17:P17"/>
+    <mergeCell ref="P22:P23"/>
     <mergeCell ref="B48:I48"/>
     <mergeCell ref="K48:P48"/>
     <mergeCell ref="V48:X48"/>

</xml_diff>